<commit_message>
GANTT updates. (KW 12 & 13)
</commit_message>
<xml_diff>
--- a/2_Documentation/GANTT/GANTT.xlsx
+++ b/2_Documentation/GANTT/GANTT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="521" documentId="13_ncr:1_{B83F1FDC-9097-4D23-B056-F10483920BA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4B08F16-AD9E-455A-BAB1-1204DB86AD78}"/>
+  <xr:revisionPtr revIDLastSave="530" documentId="13_ncr:1_{B83F1FDC-9097-4D23-B056-F10483920BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B307AC2C-BB09-4704-8C1B-0BCCBBAF1BBE}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -13,17 +13,28 @@
   <definedNames>
     <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
     <definedName name="ActualBeyond">PeriodInActual*('Project Planner'!$E1&gt;0)</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="PercentComplete">PercentCompleteBeyond*PeriodInPlan</definedName>
     <definedName name="PercentCompleteBeyond">('Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1)*('Project Planner'!$E1&gt;0))*(('Project Planner'!A$4&lt;(INT('Project Planner'!$E1+'Project Planner'!$F1*'Project Planner'!$G1)))+('Project Planner'!A$4='Project Planner'!$E1))*('Project Planner'!$G1&gt;0)</definedName>
     <definedName name="period_selected">'Project Planner'!#REF!</definedName>
     <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1-1)</definedName>
     <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$C1,'Project Planner'!$C1+'Project Planner'!$D1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -172,9 +183,6 @@
     <t>case finalization and order</t>
   </si>
   <si>
-    <t>nRF24 test and abstraction</t>
-  </si>
-  <si>
     <t>LIS2HH12 abstraction</t>
   </si>
   <si>
@@ -206,6 +214,9 @@
   </si>
   <si>
     <t>Second milestone meeting</t>
+  </si>
+  <si>
+    <t>nRF24 test and abstraction (obsolete)</t>
   </si>
 </sst>
 </file>
@@ -668,20 +679,20 @@
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Überschrift" xfId="8" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1063,20 +1074,20 @@
   </sheetPr>
   <dimension ref="B1:AA28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
-    <col min="3" max="6" width="8.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="4" customWidth="1"/>
-    <col min="8" max="25" width="4.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.59765625" customWidth="1"/>
+    <col min="2" max="2" width="22.265625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="8.3984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1328125" style="4" customWidth="1"/>
+    <col min="8" max="25" width="4.1328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="2:27" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
       <c r="B1" s="9" t="s">
         <v>12</v>
       </c>
@@ -1086,7 +1097,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="2:27" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:27" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="10"/>
       <c r="C2" s="16" t="s">
         <v>10</v>
@@ -1124,7 +1135,7 @@
       <c r="Z2" s="19"/>
       <c r="AA2" s="19"/>
     </row>
-    <row r="3" spans="2:27" s="7" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" s="7" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1176,7 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="25"/>
     </row>
-    <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="33"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -1244,7 +1255,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="20" t="s">
         <v>14</v>
       </c>
@@ -1282,7 +1293,7 @@
       <c r="X5" s="22"/>
       <c r="Y5" s="23"/>
     </row>
-    <row r="6" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="20" t="s">
         <v>15</v>
       </c>
@@ -1320,7 +1331,7 @@
       <c r="X6" s="22"/>
       <c r="Y6" s="23"/>
     </row>
-    <row r="7" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="20" t="s">
         <v>16</v>
       </c>
@@ -1358,7 +1369,7 @@
       <c r="X7" s="22"/>
       <c r="Y7" s="23"/>
     </row>
-    <row r="8" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="20" t="s">
         <v>17</v>
       </c>
@@ -1396,7 +1407,7 @@
       <c r="X8" s="22"/>
       <c r="Y8" s="23"/>
     </row>
-    <row r="9" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="20" t="s">
         <v>19</v>
       </c>
@@ -1407,13 +1418,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="21">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F9" s="21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G9" s="24">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
@@ -1434,7 +1445,7 @@
       <c r="X9" s="22"/>
       <c r="Y9" s="23"/>
     </row>
-    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="20" t="s">
         <v>18</v>
       </c>
@@ -1445,13 +1456,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="21">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F10" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
@@ -1472,7 +1483,7 @@
       <c r="X10" s="22"/>
       <c r="Y10" s="23"/>
     </row>
-    <row r="11" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="20" t="s">
         <v>20</v>
       </c>
@@ -1510,7 +1521,7 @@
       <c r="X11" s="22"/>
       <c r="Y11" s="23"/>
     </row>
-    <row r="12" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="20" t="s">
         <v>21</v>
       </c>
@@ -1548,7 +1559,7 @@
       <c r="X12" s="22"/>
       <c r="Y12" s="23"/>
     </row>
-    <row r="13" spans="2:27" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="20"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -1574,9 +1585,9 @@
       <c r="X13" s="22"/>
       <c r="Y13" s="23"/>
     </row>
-    <row r="14" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="20" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C14" s="21">
         <v>13</v>
@@ -1612,9 +1623,9 @@
       <c r="X14" s="22"/>
       <c r="Y14" s="23"/>
     </row>
-    <row r="15" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="21">
         <v>16</v>
@@ -1650,9 +1661,9 @@
       <c r="X15" s="22"/>
       <c r="Y15" s="23"/>
     </row>
-    <row r="16" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="21">
         <v>16</v>
@@ -1688,9 +1699,9 @@
       <c r="X16" s="22"/>
       <c r="Y16" s="23"/>
     </row>
-    <row r="17" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="21">
         <v>17</v>
@@ -1726,7 +1737,7 @@
       <c r="X17" s="22"/>
       <c r="Y17" s="23"/>
     </row>
-    <row r="18" spans="2:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -1752,9 +1763,9 @@
       <c r="X18" s="22"/>
       <c r="Y18" s="23"/>
     </row>
-    <row r="19" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="21">
         <v>22</v>
@@ -1790,9 +1801,9 @@
       <c r="X19" s="22"/>
       <c r="Y19" s="23"/>
     </row>
-    <row r="20" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="21">
         <v>23</v>
@@ -1828,9 +1839,9 @@
       <c r="X20" s="22"/>
       <c r="Y20" s="23"/>
     </row>
-    <row r="21" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="21">
         <v>24</v>
@@ -1866,9 +1877,9 @@
       <c r="X21" s="22"/>
       <c r="Y21" s="23"/>
     </row>
-    <row r="22" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="21">
         <v>25</v>
@@ -1904,7 +1915,7 @@
       <c r="X22" s="22"/>
       <c r="Y22" s="23"/>
     </row>
-    <row r="23" spans="2:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -1930,9 +1941,9 @@
       <c r="X23" s="22"/>
       <c r="Y23" s="23"/>
     </row>
-    <row r="24" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="21">
         <v>8</v>
@@ -1968,9 +1979,9 @@
       <c r="X24" s="22"/>
       <c r="Y24" s="23"/>
     </row>
-    <row r="25" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="21">
         <v>8</v>
@@ -2006,7 +2017,7 @@
       <c r="X25" s="22"/>
       <c r="Y25" s="23"/>
     </row>
-    <row r="26" spans="2:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="20"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -2032,9 +2043,9 @@
       <c r="X26" s="22"/>
       <c r="Y26" s="23"/>
     </row>
-    <row r="27" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="21">
         <v>14</v>
@@ -2070,9 +2081,9 @@
       <c r="X27" s="22"/>
       <c r="Y27" s="23"/>
     </row>
-    <row r="28" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:25" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="21">
         <v>21</v>

</xml_diff>